<commit_message>
test: update test data and example output
</commit_message>
<xml_diff>
--- a/data/emu.xlsx
+++ b/data/emu.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="qc" sheetId="1" r:id="rId1"/>
-    <sheet name="emu_counts" sheetId="2" r:id="rId2"/>
-    <sheet name="emu_proportions" sheetId="3" r:id="rId3"/>
+    <sheet name="emu_long" sheetId="2" r:id="rId2"/>
+    <sheet name="emu_counts" sheetId="3" r:id="rId3"/>
+    <sheet name="emu_proportions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="54">
   <si>
     <t>#filtered</t>
   </si>
@@ -75,6 +76,42 @@
     <t>species</t>
   </si>
   <si>
+    <t>abundance</t>
+  </si>
+  <si>
+    <t>estimated counts</t>
+  </si>
+  <si>
+    <t>abundance total</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Staphylococcus epidermidis</t>
+  </si>
+  <si>
+    <t>unassigned</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Leucobacter aridicollis</t>
+  </si>
+  <si>
+    <t>Bacillus sp. IHB B 7164</t>
+  </si>
+  <si>
+    <t>Bacillus megaterium</t>
+  </si>
+  <si>
     <t>genus</t>
   </si>
   <si>
@@ -91,27 +128,6 @@
   </si>
   <si>
     <t>superkingdom</t>
-  </si>
-  <si>
-    <t>Escherichia coli</t>
-  </si>
-  <si>
-    <t>Staphylococcus aureus</t>
-  </si>
-  <si>
-    <t>Staphylococcus epidermidis</t>
-  </si>
-  <si>
-    <t>Leucobacter aridicollis</t>
-  </si>
-  <si>
-    <t>Bacillus sp. IHB B 7164</t>
-  </si>
-  <si>
-    <t>Bacillus megaterium</t>
-  </si>
-  <si>
-    <t>unassigned</t>
   </si>
   <si>
     <t>Escherichia</t>
@@ -567,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>45448.48255444763</v>
+        <v>45552.44911822711</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -599,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>45448.48255444763</v>
+        <v>45552.44911822711</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -631,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>45448.48255444763</v>
+        <v>45552.44911822711</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -663,7 +679,7 @@
         <v>0.5326666666666666</v>
       </c>
       <c r="F5" s="2">
-        <v>45448.48255444763</v>
+        <v>45552.44911822711</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -695,7 +711,7 @@
         <v>0.9</v>
       </c>
       <c r="F6" s="2">
-        <v>45448.48255444763</v>
+        <v>45552.44911822711</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -717,7 +733,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -731,227 +747,329 @@
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2700</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>2700</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2533</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>2533</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2791</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>2791</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.8848560700876095</v>
+      </c>
+      <c r="D11">
+        <v>1414</v>
+      </c>
+      <c r="E11">
+        <v>0.8848560700876095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>0.0677402327456906</v>
+      </c>
+      <c r="D12">
+        <v>108.2488919276137</v>
+      </c>
+      <c r="E12">
+        <v>0.06774023274569065</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13">
+        <v>0.0474036971666998</v>
+      </c>
+      <c r="D13">
+        <v>75.75110807238636</v>
+      </c>
+      <c r="E13">
+        <v>0.04740369716669985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>1598</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>0.4444444444444444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>0.3081387123397617</v>
+      </c>
+      <c r="D17">
+        <v>2.773248411057855</v>
+      </c>
+      <c r="E17">
+        <v>0.3081387123397617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18">
+        <v>0.2474168432157938</v>
+      </c>
+      <c r="D18">
+        <v>2.226751588942145</v>
+      </c>
+      <c r="E18">
+        <v>0.2474168432157938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2">
-        <v>2533</v>
-      </c>
-      <c r="K2">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3">
-        <v>2791</v>
-      </c>
-      <c r="K3">
-        <v>75.75110807238636</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4">
-        <v>2700</v>
-      </c>
-      <c r="K4">
-        <v>108.2488919276137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6">
-        <v>2.773248411057855</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" t="s">
-        <v>48</v>
-      </c>
-      <c r="L7">
-        <v>2.226751588942145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -980,22 +1098,22 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
@@ -1015,89 +1133,89 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2533</v>
       </c>
       <c r="K2">
-        <v>0.8848560700876095</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>2791</v>
       </c>
       <c r="K3">
-        <v>0.0474036971666998</v>
+        <v>75.75110807238636</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>2700</v>
       </c>
       <c r="K4">
-        <v>0.0677402327456906</v>
+        <v>108.2488919276137</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1105,25 +1223,25 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L5">
-        <v>0.4444444444444444</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1131,25 +1249,25 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L6">
-        <v>0.3081387123397617</v>
+        <v>2.773248411057855</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1157,22 +1275,266 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7">
+        <v>2.226751588942145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.8848560700876095</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.0474036971666998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.0677402327456906</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5">
+        <v>0.4444444444444444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6">
+        <v>0.3081387123397617</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="L7">
         <v>0.2474168432157938</v>
@@ -1180,7 +1542,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>

<commit_message>
feat: new column (%) in report
</commit_message>
<xml_diff>
--- a/data/emu.xlsx
+++ b/data/emu.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="55">
   <si>
     <t>#filtered</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>abundance total</t>
+  </si>
+  <si>
+    <t>% total</t>
   </si>
   <si>
     <t>Sample</t>
@@ -583,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>45552.44911822711</v>
+        <v>45642.47677915011</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -615,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>45552.44911822711</v>
+        <v>45642.47677915011</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -647,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>45552.44911822711</v>
+        <v>45642.47677915011</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -679,7 +682,7 @@
         <v>0.5326666666666666</v>
       </c>
       <c r="F5" s="2">
-        <v>45552.44911822711</v>
+        <v>45642.47677915011</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -711,7 +714,7 @@
         <v>0.9</v>
       </c>
       <c r="F6" s="2">
-        <v>45552.44911822711</v>
+        <v>45642.47677915011</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -733,7 +736,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -747,9 +750,9 @@
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
@@ -763,13 +766,16 @@
       <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -780,13 +786,16 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -797,13 +806,16 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>2700</v>
@@ -811,13 +823,16 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -828,13 +843,16 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -845,13 +863,16 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>2533</v>
@@ -859,13 +880,16 @@
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -876,13 +900,16 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -893,13 +920,16 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10">
         <v>2791</v>
@@ -907,13 +937,16 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>0.8848560700876095</v>
@@ -924,13 +957,16 @@
       <c r="E11">
         <v>0.8848560700876095</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <v>88.48560700876095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12">
         <v>0.0677402327456906</v>
@@ -941,13 +977,16 @@
       <c r="E12">
         <v>0.06774023274569065</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <v>6.774023274569065</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0.0474036971666998</v>
@@ -958,13 +997,16 @@
       <c r="E13">
         <v>0.04740369716669985</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <v>4.740369716669985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -975,13 +1017,16 @@
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>1598</v>
@@ -989,13 +1034,16 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>0.4444444444444444</v>
@@ -1006,13 +1054,16 @@
       <c r="E16">
         <v>0.4444444444444444</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>44.44444444444444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>0.3081387123397617</v>
@@ -1023,13 +1074,16 @@
       <c r="E17">
         <v>0.3081387123397617</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>30.81387123397617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>0.2474168432157938</v>
@@ -1040,13 +1094,16 @@
       <c r="E18">
         <v>0.2474168432157938</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>24.74168432157938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1057,19 +1114,25 @@
       <c r="E19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D20">
         <v>9</v>
       </c>
       <c r="E20">
         <v>1</v>
+      </c>
+      <c r="F20">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1098,22 +1161,22 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
@@ -1133,25 +1196,25 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I2">
         <v>2533</v>
@@ -1162,25 +1225,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J3">
         <v>2791</v>
@@ -1191,25 +1254,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>2700</v>
@@ -1220,25 +1283,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -1246,25 +1309,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L6">
         <v>2.773248411057855</v>
@@ -1272,25 +1335,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L7">
         <v>2.226751588942145</v>
@@ -1298,7 +1361,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1342,22 +1405,22 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
@@ -1377,25 +1440,25 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1406,25 +1469,25 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J3">
         <v>1</v>
@@ -1435,25 +1498,25 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1464,25 +1527,25 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L5">
         <v>0.4444444444444444</v>
@@ -1490,25 +1553,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L6">
         <v>0.3081387123397617</v>
@@ -1516,25 +1579,25 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L7">
         <v>0.2474168432157938</v>
@@ -1542,7 +1605,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>

<commit_message>
feat: report formatting - cell width, rounding and borders
</commit_message>
<xml_diff>
--- a/data/emu.xlsx
+++ b/data/emu.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="57">
   <si>
     <t>#filtered</t>
   </si>
@@ -34,6 +34,9 @@
     <t>report_date</t>
   </si>
   <si>
+    <t>github_version</t>
+  </si>
+  <si>
     <t>emu_image</t>
   </si>
   <si>
@@ -61,7 +64,10 @@
     <t>barcode05</t>
   </si>
   <si>
-    <t>emu:2024-05-13</t>
+    <t>v.0.3.0</t>
+  </si>
+  <si>
+    <t>emu:2024-12-16</t>
   </si>
   <si>
     <t>3.4.5</t>
@@ -216,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -224,14 +230,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +542,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -538,9 +554,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -568,10 +587,13 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>2700</v>
@@ -586,24 +608,27 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>45642.47677915011</v>
+        <v>45642.60027498117</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>2533</v>
@@ -618,24 +643,27 @@
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>45642.47677915011</v>
+        <v>45642.60027498117</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>2791</v>
@@ -650,24 +678,27 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>45642.47677915011</v>
+        <v>45642.60027498117</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>3000</v>
@@ -679,27 +710,30 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.5326666666666666</v>
+        <v>0.53</v>
       </c>
       <c r="F5" s="2">
-        <v>45642.47677915011</v>
+        <v>45642.60027498117</v>
       </c>
       <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -714,19 +748,22 @@
         <v>0.9</v>
       </c>
       <c r="F6" s="2">
-        <v>45642.47677915011</v>
+        <v>45642.60027498117</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -748,34 +785,35 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -792,10 +830,10 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -810,29 +848,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
+    <row r="4" spans="1:6" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3">
         <v>2700</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -849,10 +887,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -867,29 +905,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7">
+    <row r="7" spans="1:6" s="3" customFormat="1">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3">
         <v>2533</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -906,10 +944,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -924,89 +962,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10">
+    <row r="10" spans="1:6" s="3" customFormat="1">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3">
         <v>2791</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11">
-        <v>0.8848560700876095</v>
+        <v>0.88</v>
       </c>
       <c r="D11">
         <v>1414</v>
       </c>
       <c r="E11">
-        <v>0.8848560700876095</v>
+        <v>0.88</v>
       </c>
       <c r="F11">
-        <v>88.48560700876095</v>
+        <v>88.48999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>0.0677402327456906</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D12">
-        <v>108.2488919276137</v>
+        <v>108.25</v>
       </c>
       <c r="E12">
-        <v>0.06774023274569065</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F12">
-        <v>6.774023274569065</v>
+        <v>6.77</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13">
-        <v>0.0474036971666998</v>
+        <v>0.05</v>
       </c>
       <c r="D13">
-        <v>75.75110807238636</v>
+        <v>75.75</v>
       </c>
       <c r="E13">
-        <v>0.04740369716669985</v>
+        <v>0.05</v>
       </c>
       <c r="F13">
-        <v>4.740369716669985</v>
+        <v>4.74</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1021,89 +1059,89 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15">
+    <row r="15" spans="1:6" s="3" customFormat="1">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3">
         <v>1598</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>0.4444444444444444</v>
+        <v>0.44</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16">
-        <v>0.4444444444444444</v>
+        <v>0.44</v>
       </c>
       <c r="F16">
-        <v>44.44444444444444</v>
+        <v>44.44</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17">
-        <v>0.3081387123397617</v>
+        <v>0.31</v>
       </c>
       <c r="D17">
-        <v>2.773248411057855</v>
+        <v>2.77</v>
       </c>
       <c r="E17">
-        <v>0.3081387123397617</v>
+        <v>0.31</v>
       </c>
       <c r="F17">
-        <v>30.81387123397617</v>
+        <v>30.81</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18">
-        <v>0.2474168432157938</v>
+        <v>0.25</v>
       </c>
       <c r="D18">
-        <v>2.226751588942145</v>
+        <v>2.23</v>
       </c>
       <c r="E18">
-        <v>0.2474168432157938</v>
+        <v>0.25</v>
       </c>
       <c r="F18">
-        <v>24.74168432157938</v>
+        <v>24.74</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1118,20 +1156,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20">
+    <row r="20" spans="1:6" s="3" customFormat="1">
+      <c r="A20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3">
         <v>9</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
         <v>100</v>
       </c>
     </row>
@@ -1158,63 +1196,63 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I2">
         <v>2533</v>
@@ -1225,83 +1263,83 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J3">
         <v>2791</v>
       </c>
       <c r="K3">
-        <v>75.75110807238636</v>
+        <v>75.75</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H4">
         <v>2700</v>
       </c>
       <c r="K4">
-        <v>108.2488919276137</v>
+        <v>108.25</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -1309,59 +1347,59 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L6">
-        <v>2.773248411057855</v>
+        <v>2.77</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L7">
-        <v>2.226751588942145</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1402,210 +1440,210 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.8848560700876095</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3">
-        <v>0.0474036971666998</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0.0677402327456906</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L5">
-        <v>0.4444444444444444</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L6">
-        <v>0.3081387123397617</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L7">
-        <v>0.2474168432157938</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>

<commit_message>
feat: make taxa blue if passing min_counts_taxa and min_abund_tot even if total < min_reads, update matching test data
</commit_message>
<xml_diff>
--- a/data/emu.xlsx
+++ b/data/emu.xlsx
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>45750.68891013654</v>
+        <v>45758.65994086969</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -981,13 +981,13 @@
         <v>110</v>
       </c>
       <c r="C6">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E6">
-        <v>0.08</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -1242,7 +1242,7 @@
         <v>55</v>
       </c>
       <c r="C12" s="5">
-        <v>0.92</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5">
         <v>1500</v>
@@ -1262,7 +1262,7 @@
         <v>59</v>
       </c>
       <c r="C13">
-        <v>0.06</v>
+        <v>0.74</v>
       </c>
       <c r="D13">
         <v>100</v>
@@ -1282,7 +1282,7 @@
         <v>54</v>
       </c>
       <c r="C14">
-        <v>0.02</v>
+        <v>0.19</v>
       </c>
       <c r="D14">
         <v>25</v>
@@ -1302,7 +1302,7 @@
         <v>58</v>
       </c>
       <c r="C15">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D15">
         <v>10</v>
@@ -1331,24 +1331,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:6" s="3" customFormat="1">
+      <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17">
-        <v>0.95</v>
-      </c>
-      <c r="D17">
-        <v>100</v>
-      </c>
-      <c r="E17">
-        <v>0.92</v>
-      </c>
-      <c r="F17">
-        <v>91.73999999999999</v>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="D17" s="3">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.48</v>
+      </c>
+      <c r="F17" s="3">
+        <v>47.62</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1356,19 +1356,19 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C18">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="E18">
-        <v>0.04</v>
+        <v>0.48</v>
       </c>
       <c r="F18">
-        <v>3.67</v>
+        <v>47.62</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1379,7 +1379,7 @@
         <v>61</v>
       </c>
       <c r="C19">
-        <v>0.31</v>
+        <v>0.05</v>
       </c>
       <c r="D19">
         <v>2.77</v>
@@ -1388,7 +1388,7 @@
         <v>0.03</v>
       </c>
       <c r="F19">
-        <v>2.54</v>
+        <v>2.64</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1399,7 +1399,7 @@
         <v>62</v>
       </c>
       <c r="C20">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
       <c r="D20">
         <v>2.23</v>
@@ -1408,7 +1408,7 @@
         <v>0.02</v>
       </c>
       <c r="F20">
-        <v>2.04</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1">
@@ -1419,7 +1419,7 @@
         <v>56</v>
       </c>
       <c r="D21" s="6">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E21" s="6">
         <v>1</v>
@@ -1634,7 +1634,7 @@
         <v>90</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1706,7 +1706,7 @@
         <v>1500</v>
       </c>
       <c r="L9">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>0.02</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1860,7 +1860,7 @@
         <v>0.95</v>
       </c>
       <c r="K4">
-        <v>0.01</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1889,7 +1889,7 @@
         <v>0.05</v>
       </c>
       <c r="K5">
-        <v>0.06</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1915,7 +1915,7 @@
         <v>90</v>
       </c>
       <c r="L6">
-        <v>0.44</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1941,7 +1941,7 @@
         <v>90</v>
       </c>
       <c r="L7">
-        <v>0.31</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1967,7 +1967,7 @@
         <v>90</v>
       </c>
       <c r="L8">
-        <v>0.25</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1984,10 +1984,10 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.92</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0.95</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>